<commit_message>
Updated registration form with subform
</commit_message>
<xml_diff>
--- a/appGreece/config/tables/registration/forms/registration/registration.xlsx
+++ b/appGreece/config/tables/registration/forms/registration/registration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="80" windowWidth="44040" windowHeight="24600" tabRatio="994" activeTab="9"/>
+    <workbookView xWindow="680" yWindow="220" windowWidth="49720" windowHeight="24760" tabRatio="994"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,9 @@
     <sheet name="table_specific_translations" sheetId="3" r:id="rId3"/>
     <sheet name="model" sheetId="4" r:id="rId4"/>
     <sheet name="choices" sheetId="6" r:id="rId5"/>
-    <sheet name="calculates" sheetId="7" r:id="rId6"/>
-    <sheet name="properties" sheetId="8" r:id="rId7"/>
-    <sheet name="queries" sheetId="9" r:id="rId8"/>
-    <sheet name="prompt_types" sheetId="10" r:id="rId9"/>
-    <sheet name="initial" sheetId="11" r:id="rId10"/>
+    <sheet name="properties" sheetId="8" r:id="rId6"/>
+    <sheet name="queries" sheetId="9" r:id="rId7"/>
+    <sheet name="initial" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="123">
   <si>
     <t>clause</t>
   </si>
@@ -72,9 +70,6 @@
     <t>verify_user</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
     <t>date_screened</t>
   </si>
   <si>
@@ -93,45 +88,15 @@
     <t>string</t>
   </si>
   <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>What is your first name?</t>
-  </si>
-  <si>
-    <t>First name</t>
-  </si>
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>What is your last Name?</t>
-  </si>
-  <si>
-    <t>Last name</t>
-  </si>
-  <si>
     <t>first_last_name</t>
   </si>
   <si>
-    <t>data('first_name') + " " + data('last_name')</t>
-  </si>
-  <si>
     <t>end screen</t>
   </si>
   <si>
-    <t>id_type</t>
-  </si>
-  <si>
-    <t>What type of ID do you have?</t>
-  </si>
-  <si>
     <t>id_number</t>
   </si>
   <si>
-    <t>What is your ID number?</t>
-  </si>
-  <si>
     <t>mobile_provider</t>
   </si>
   <si>
@@ -150,48 +115,12 @@
     <t>number</t>
   </si>
   <si>
-    <t>async_assign_single_string</t>
-  </si>
-  <si>
-    <t>verify_user_query</t>
-  </si>
-  <si>
-    <t>if</t>
-  </si>
-  <si>
-    <t>(data('verify_user') !== null)</t>
-  </si>
-  <si>
     <t>note</t>
   </si>
   <si>
-    <t>end if</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>birth_date</t>
-  </si>
-  <si>
-    <t>What is your date of birth?</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>calculates.age()</t>
-  </si>
-  <si>
     <t>select_one</t>
   </si>
   <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>What is your gender?</t>
-  </si>
-  <si>
     <t>genders</t>
   </si>
   <si>
@@ -372,12 +301,6 @@
     <t>Site D</t>
   </si>
   <si>
-    <t>calculation_name</t>
-  </si>
-  <si>
-    <t>(function() {var ageDifMs = Date.now() - data('birth_date').getTime();var ageDate = new Date(ageDifMs);var years = Math.abs(ageDate.getUTCFullYear() - 1970);var months = ageDate.getUTCMonth();var days = ageDate.getUTCDate();var daysOfMonth = [31, 28, 31, 30, 31, 30, 31, 31, 30, 31, 30, 31];var daysInCurrYear = 0;for (var i = 0; i &lt; months; i++) {daysInCurrYear += daysOfMonth[i];}daysInCurrYear += days;var age = years + (daysInCurrYear / 365.0);return age;})()</t>
-  </si>
-  <si>
     <t>partition</t>
   </si>
   <si>
@@ -426,9 +349,6 @@
     <t>selectionArgs</t>
   </si>
   <si>
-    <t>fieldName</t>
-  </si>
-  <si>
     <t>newRowInitialElementKeyToValueMap</t>
   </si>
   <si>
@@ -438,40 +358,49 @@
     <t>linked_table</t>
   </si>
   <si>
-    <t>_savepoint_type = ? and first_last_name = ? and id_number = ? and telephone = ?</t>
-  </si>
-  <si>
-    <t>['COMPLETE', data('first_last_name'), data('id_number'), data('telephone')]</t>
-  </si>
-  <si>
     <t>{}</t>
   </si>
   <si>
-    <t>prompt_type_name</t>
-  </si>
-  <si>
-    <t>async_assign_max</t>
-  </si>
-  <si>
-    <t>async_assign_min</t>
-  </si>
-  <si>
-    <t>async_assign_avg</t>
-  </si>
-  <si>
-    <t>async_assign_sum</t>
-  </si>
-  <si>
-    <t>async_assign_total</t>
-  </si>
-  <si>
-    <t>async_assign_count</t>
-  </si>
-  <si>
-    <t>User {{data.verify_user}} already exists.  Continue if you are sure.  Otherwise, Ignore Changes + Exit.</t>
-  </si>
-  <si>
     <t>isSessionVariable</t>
+  </si>
+  <si>
+    <t>registrationMember</t>
+  </si>
+  <si>
+    <t>beneficiary_code = ?</t>
+  </si>
+  <si>
+    <t>[ data('beneficiary_code') ]</t>
+  </si>
+  <si>
+    <t>{beneficiary_code: data('beneficiary_code')}</t>
+  </si>
+  <si>
+    <t>Household Members Section:</t>
+  </si>
+  <si>
+    <t>reg_members</t>
+  </si>
+  <si>
+    <t>Make a list of all individuals who normally live in this household</t>
+  </si>
+  <si>
+    <t>consent_signature</t>
+  </si>
+  <si>
+    <t>tent_caravan</t>
+  </si>
+  <si>
+    <t>Tent/Caravan code:</t>
+  </si>
+  <si>
+    <t>signature</t>
+  </si>
+  <si>
+    <t>"Data collected will be used to provide you with easier access to the Red Cross services. The information gathered during this interview will stay with Red Cross and will be stored in a Spanish Red Cross server. No sensitive data will be shared with any other person or organization. 
+If you agree with this process and this use of information, we will proceed with the interview.
+We inform you that you can exercise, at any time, the rights of access, rectification, cancellation and opposition, directing a letter to: Cruz Roja Española, Secretaría General, Avenida Reina Victoria, 26, 28003 Madrid, or to the email address: odksupport@cruzroja.es, previous accreditation of your identity.
+Consent signature (In the case of a minor, the legal guardian will sign in its place)"</t>
   </si>
 </sst>
 </file>
@@ -630,7 +559,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -638,8 +567,28 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -651,8 +600,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -660,18 +607,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -695,20 +633,43 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1106,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMI34"/>
+  <dimension ref="A1:AMI23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" x14ac:dyDescent="0"/>
@@ -1118,8 +1079,8 @@
     <col min="2" max="2" width="29.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="33.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="35.83203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="44.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="32.33203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="71.5" style="4" customWidth="1"/>
+    <col min="6" max="6" width="45.1640625" style="5" customWidth="1"/>
     <col min="7" max="7" width="34.5" style="5" customWidth="1"/>
     <col min="8" max="8" width="34.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="30.6640625" style="1" customWidth="1"/>
@@ -1169,16 +1130,16 @@
         <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
-      <c r="G2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="G2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
       <c r="K2"/>
     </row>
     <row r="3" spans="1:11">
@@ -1187,13 +1148,14 @@
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="5" t="s">
+      <c r="D3" s="13" t="s">
         <v>15</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
@@ -1203,17 +1165,17 @@
     <row r="4" spans="1:11">
       <c r="A4"/>
       <c r="B4"/>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="14" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H4"/>
       <c r="I4"/>
@@ -1221,155 +1183,125 @@
       <c r="K4"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5"/>
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="B5"/>
-      <c r="C5" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
       <c r="H5"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
     </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
+    <row r="6" spans="1:11" ht="409">
+      <c r="A6"/>
       <c r="B6"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
+      <c r="C6" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
       <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
       <c r="K6"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7"/>
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="B7"/>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7"/>
       <c r="I7"/>
       <c r="J7"/>
-      <c r="K7" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="K7"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8"/>
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="B8"/>
-      <c r="C8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8"/>
+      <c r="F8" s="12"/>
       <c r="H8"/>
       <c r="I8"/>
       <c r="J8"/>
-      <c r="K8" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="12"/>
       <c r="H9"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="A10"/>
       <c r="B10"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="H10"/>
       <c r="I10"/>
-      <c r="J10"/>
+      <c r="J10" t="s">
+        <v>27</v>
+      </c>
       <c r="K10"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B11"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
+      <c r="F11" s="12"/>
       <c r="H11"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="14"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13"/>
-      <c r="B13"/>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>31</v>
@@ -1377,381 +1309,149 @@
       <c r="E13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-      <c r="K13" s="1" t="b">
+      <c r="F13" s="12"/>
+      <c r="H13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14"/>
+      <c r="C14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15"/>
+      <c r="C15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" s="1" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14"/>
-      <c r="F14" s="14"/>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
-      <c r="J14"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15"/>
-      <c r="F15" s="14"/>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15"/>
-    </row>
     <row r="16" spans="1:11">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="14"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-      <c r="K16"/>
+      <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17"/>
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="B17"/>
-      <c r="C17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
       <c r="H17"/>
       <c r="I17"/>
-      <c r="J17" t="s">
-        <v>38</v>
-      </c>
+      <c r="J17"/>
       <c r="K17"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18"/>
       <c r="B18"/>
-      <c r="C18" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="23"/>
-      <c r="G18"/>
-      <c r="H18" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="C18" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
       <c r="K18"/>
     </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="1" t="s">
-        <v>28</v>
-      </c>
+    <row r="19" spans="1:11" ht="46">
+      <c r="A19"/>
       <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19" s="24"/>
-      <c r="H19"/>
+      <c r="C19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="H19" t="s">
+        <v>116</v>
+      </c>
       <c r="I19"/>
       <c r="J19"/>
-      <c r="K19"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="27"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20" s="24"/>
+        <v>20</v>
+      </c>
+      <c r="B20"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="12"/>
       <c r="H20"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21"/>
       <c r="C21" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21"/>
-      <c r="I21"/>
-      <c r="J21"/>
-      <c r="K21" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22"/>
       <c r="C22" s="2" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="14"/>
-      <c r="H22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K22" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="14"/>
-    </row>
-    <row r="24" spans="1:11" ht="46">
-      <c r="A24" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="24"/>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24" s="24"/>
-      <c r="H24"/>
-      <c r="I24"/>
-      <c r="J24"/>
-      <c r="K24"/>
-    </row>
-    <row r="25" spans="1:11" ht="69">
-      <c r="A25"/>
-      <c r="C25" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25"/>
-      <c r="E25" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25"/>
-      <c r="I25"/>
-      <c r="J25"/>
-      <c r="K25"/>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="1" t="s">
+      <c r="E23" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="C26" s="27"/>
-      <c r="D26"/>
-      <c r="E26"/>
-      <c r="F26"/>
-      <c r="G26" s="24"/>
-      <c r="H26"/>
-      <c r="I26"/>
-      <c r="J26"/>
-      <c r="K26"/>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="14"/>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28"/>
-      <c r="C28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H28"/>
-      <c r="I28"/>
-      <c r="J28"/>
-      <c r="K28"/>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29"/>
-      <c r="C29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F29" s="14"/>
-      <c r="H29" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K29"/>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30"/>
-      <c r="C30" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="K30"/>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31"/>
-      <c r="C31" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K31" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32"/>
-      <c r="D32"/>
-      <c r="E32"/>
-    </row>
-    <row r="33" spans="3:5">
-      <c r="C33" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="3:5">
-      <c r="C34" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
-    <col min="4" max="4" width="49.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-    </row>
-    <row r="3" spans="1:4" ht="30">
-      <c r="A3" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33" t="s">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1765,74 +1465,73 @@
   <dimension ref="A1:AMK6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="28"/>
-    <col min="2" max="2" width="8.83203125" style="29"/>
+    <col min="1" max="1" width="25.1640625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="38.5" style="20" customWidth="1"/>
     <col min="3" max="1025" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>69</v>
+      <c r="A1" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>46</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>72</v>
+      <c r="A2" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>49</v>
       </c>
       <c r="C2"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="29">
-        <v>20160805</v>
+      <c r="A3" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="20">
+        <v>20170530</v>
       </c>
       <c r="C3"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>72</v>
+      <c r="A4" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>49</v>
       </c>
       <c r="C4"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5"/>
+      <c r="A5" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="C5" s="1" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>26</v>
+      <c r="A6" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1850,88 +1549,92 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="41" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1947,191 +1650,144 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK21"/>
+  <dimension ref="A1:AMK15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="20.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="53.1640625" style="3" customWidth="1"/>
-    <col min="3" max="1025" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="22.83203125" style="1" customWidth="1"/>
+    <col min="4" max="1025" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="23" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>146</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>33</v>
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>19</v>
+        <v>121</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="1" t="b">
-        <v>1</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2147,89 +1803,94 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30">
-      <c r="A1" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>70</v>
+    <row r="1" spans="1:3">
+      <c r="A1" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2245,31 +1906,66 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="44.1640625" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="165">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>114</v>
+    <row r="1" spans="1:5">
+      <c r="A1" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2285,68 +1981,79 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="31.83203125" customWidth="1"/>
+    <col min="6" max="6" width="39.33203125" customWidth="1"/>
+    <col min="7" max="7" width="43.5" customWidth="1"/>
+    <col min="8" max="8" width="36.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="B1" s="35" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="35" t="s">
-        <v>117</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>122</v>
-      </c>
-      <c r="D3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E3" s="35" t="s">
-        <v>124</v>
+      <c r="B2" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2357,166 +2064,51 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="5" max="5" width="31.83203125" customWidth="1"/>
-    <col min="6" max="6" width="39.33203125" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" customWidth="1"/>
-    <col min="8" max="8" width="27.5" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="4" max="4" width="49.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30">
-      <c r="A1" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="D1" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>129</v>
-      </c>
-      <c r="F1" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" s="39" t="s">
-        <v>131</v>
-      </c>
-      <c r="H1" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="I1" s="40" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="45">
-      <c r="A2" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>134</v>
-      </c>
-      <c r="C2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="41" t="s">
-        <v>135</v>
-      </c>
-      <c r="F2" s="41" t="s">
-        <v>136</v>
-      </c>
-      <c r="G2" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="I2" s="42" t="s">
-        <v>137</v>
+    <row r="1" spans="1:4">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+    </row>
+    <row r="3" spans="1:4" ht="30">
+      <c r="A3" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:2" ht="45">
-      <c r="A1" s="33" t="s">
-        <v>138</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="45">
-      <c r="A2" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="30">
-      <c r="A3" s="33" t="s">
-        <v>140</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30">
-      <c r="A4" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="45">
-      <c r="A5" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="45">
-      <c r="A6" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="45">
-      <c r="A7" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="45">
-      <c r="A8" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
New forms for registration
</commit_message>
<xml_diff>
--- a/appGreece/config/tables/registration/forms/registration/registration.xlsx
+++ b/appGreece/config/tables/registration/forms/registration/registration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6760" yWindow="3240" windowWidth="49720" windowHeight="24780" tabRatio="994"/>
+    <workbookView xWindow="4660" yWindow="6400" windowWidth="30740" windowHeight="17820" tabRatio="994"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="119">
   <si>
     <t>clause</t>
   </si>
@@ -272,30 +272,6 @@
   </si>
   <si>
     <t>Female</t>
-  </si>
-  <si>
-    <t>a0</t>
-  </si>
-  <si>
-    <t>Site A</t>
-  </si>
-  <si>
-    <t>a1</t>
-  </si>
-  <si>
-    <t>Site B</t>
-  </si>
-  <si>
-    <t>a2</t>
-  </si>
-  <si>
-    <t>Site C</t>
-  </si>
-  <si>
-    <t>a3</t>
-  </si>
-  <si>
-    <t>Site D</t>
   </si>
   <si>
     <t>partition</t>
@@ -398,6 +374,21 @@
 If you agree with this process and this use of information, we will proceed with the interview.
 We inform you that you can exercise, at any time, the rights of access, rectification, cancellation and opposition, directing a letter to: Cruz Roja Española, Secretaría General, Avenida Reina Victoria, 26, 28003 Madrid, or to the email address: odksupport@cruzroja.es, previous accreditation of your identity.
 Consent signature (In the case of a minor, the legal guardian will sign in its place)"</t>
+  </si>
+  <si>
+    <t>Ritsona</t>
+  </si>
+  <si>
+    <t>Skaramagas</t>
+  </si>
+  <si>
+    <t>Nea Kavala</t>
+  </si>
+  <si>
+    <t>Softex</t>
+  </si>
+  <si>
+    <t>Athens</t>
   </si>
 </sst>
 </file>
@@ -556,8 +547,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -646,7 +639,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -663,6 +656,7 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -679,6 +673,7 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1078,8 +1073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMI22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" x14ac:dyDescent="0"/>
@@ -1094,7 +1089,8 @@
     <col min="8" max="8" width="34.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="30.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="29.1640625" style="1" customWidth="1"/>
-    <col min="11" max="1023" width="8.83203125" style="1"/>
+    <col min="11" max="11" width="21.33203125" style="1" customWidth="1"/>
+    <col min="12" max="1023" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1128,7 +1124,7 @@
       <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1210,13 +1206,13 @@
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6" s="14" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -1322,7 +1318,9 @@
       <c r="H13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K13"/>
+      <c r="K13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14"/>
@@ -1387,7 +1385,7 @@
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="16" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
@@ -1400,16 +1398,16 @@
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="E19" s="18" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H19" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="I19"/>
       <c r="J19"/>
@@ -1443,12 +1441,15 @@
         <v>18</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="F22" s="12"/>
+      <c r="K22" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1673,7 +1674,7 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1777,10 +1778,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1788,7 +1789,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1804,10 +1805,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1855,10 +1856,10 @@
         <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1866,10 +1867,10 @@
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1877,10 +1878,10 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1888,15 +1889,26 @@
         <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1920,13 +1932,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="26" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>2</v>
@@ -1937,36 +1949,36 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="26" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2002,54 +2014,54 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="29" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F1" s="30" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="24" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="H2" s="32" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Convert app to pre-populate metadata fields
</commit_message>
<xml_diff>
--- a/appGreece/config/tables/registration/forms/registration/registration.xlsx
+++ b/appGreece/config/tables/registration/forms/registration/registration.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/redcross/app-designer/appGreece/config/tables/registration/forms/registration/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="6400" windowWidth="30740" windowHeight="17820" tabRatio="994" activeTab="2"/>
+    <workbookView xWindow="4820" yWindow="3240" windowWidth="34900" windowHeight="19500" tabRatio="994" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -21,13 +16,13 @@
     <sheet name="queries" sheetId="9" r:id="rId7"/>
     <sheet name="initial" sheetId="11" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -354,9 +349,6 @@
     <t>[ data('beneficiary_code') ]</t>
   </si>
   <si>
-    <t>{beneficiary_code: data('beneficiary_code')}</t>
-  </si>
-  <si>
     <t>Household Members Section:</t>
   </si>
   <si>
@@ -514,6 +506,9 @@
   </si>
   <si>
     <t>text.greek</t>
+  </si>
+  <si>
+    <t>{beneficiary_code: data('beneficiary_code'), _group_modify: 'hardcodedTestGroup'}</t>
   </si>
 </sst>
 </file>
@@ -1216,7 +1211,7 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="29.5" style="1" customWidth="1"/>
@@ -1231,7 +1226,7 @@
     <col min="11" max="11" width="21.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1266,7 +1261,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2" s="2" t="s">
@@ -1285,7 +1280,7 @@
       <c r="J2"/>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3" s="2" t="s">
@@ -1305,7 +1300,7 @@
       <c r="J3"/>
       <c r="K3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4" s="14" t="s">
@@ -1325,7 +1320,7 @@
       <c r="J4"/>
       <c r="K4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1340,17 +1335,17 @@
       <c r="J5"/>
       <c r="K5"/>
     </row>
-    <row r="6" spans="1:11" ht="409" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="409">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="34" t="s">
         <v>112</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="E6" s="34" t="s">
-        <v>113</v>
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -1359,7 +1354,7 @@
       <c r="J6"/>
       <c r="K6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -1374,7 +1369,7 @@
       <c r="J7"/>
       <c r="K7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -1384,7 +1379,7 @@
       <c r="I8"/>
       <c r="J8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9" s="2" t="s">
@@ -1402,7 +1397,7 @@
       <c r="J9"/>
       <c r="K9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10" s="2" t="s">
@@ -1424,7 +1419,7 @@
       </c>
       <c r="K10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1435,13 +1430,13 @@
       <c r="J11"/>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11">
       <c r="A13"/>
       <c r="C13" s="2" t="s">
         <v>29</v>
@@ -1460,7 +1455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11">
       <c r="A14"/>
       <c r="C14" s="2" t="s">
         <v>18</v>
@@ -1476,7 +1471,7 @@
       </c>
       <c r="K14"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11">
       <c r="A15"/>
       <c r="C15" s="2" t="s">
         <v>37</v>
@@ -1495,13 +1490,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1516,14 +1511,14 @@
       <c r="J17"/>
       <c r="K17"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11">
       <c r="B18"/>
       <c r="C18" s="14" t="s">
         <v>28</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
@@ -1532,25 +1527,25 @@
       <c r="J18"/>
       <c r="K18"/>
     </row>
-    <row r="19" spans="1:11" ht="48" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="46">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19" s="2" t="s">
         <v>99</v>
       </c>
       <c r="D19" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>108</v>
-      </c>
       <c r="H19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I19"/>
       <c r="J19"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -1562,7 +1557,7 @@
       <c r="J20"/>
       <c r="K20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11">
       <c r="C21" s="2" t="s">
         <v>41</v>
       </c>
@@ -1573,16 +1568,16 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11">
       <c r="A22"/>
       <c r="C22" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="F22" s="12"/>
       <c r="K22" s="1" t="b">
@@ -1592,6 +1587,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1603,14 +1603,14 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25.1640625" style="19" customWidth="1"/>
     <col min="2" max="2" width="38.5" style="20" customWidth="1"/>
     <col min="3" max="3" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="21" t="s">
         <v>44</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="19" t="s">
         <v>47</v>
       </c>
@@ -1630,7 +1630,7 @@
       </c>
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="19" t="s">
         <v>49</v>
       </c>
@@ -1639,7 +1639,7 @@
       </c>
       <c r="C3"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="19" t="s">
         <v>50</v>
       </c>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="19" t="s">
         <v>51</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="19" t="s">
         <v>53</v>
       </c>
@@ -1667,6 +1667,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1674,17 +1679,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26.5" customWidth="1"/>
     <col min="2" max="3" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1692,19 +1697,19 @@
         <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" t="s">
         <v>146</v>
-      </c>
-      <c r="E1" t="s">
-        <v>147</v>
       </c>
       <c r="F1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="17">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1712,19 +1717,19 @@
         <v>36</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D2" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="F2" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="35" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" ht="17">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1732,19 +1737,19 @@
         <v>57</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D3" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="F3" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F3" s="35" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:6" ht="17">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -1752,19 +1757,19 @@
         <v>59</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D4" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="F4" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="F4" s="35" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:6" ht="17">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1772,19 +1777,19 @@
         <v>60</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D5" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="F5" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="F5" s="35" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:6" ht="17">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1792,19 +1797,19 @@
         <v>61</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D6" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="F6" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="F6" s="35" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" ht="17">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -1812,19 +1817,19 @@
         <v>63</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D7" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="E7" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="F7" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="F7" s="35" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:6" ht="17">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -1832,19 +1837,19 @@
         <v>65</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D8" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="E8" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="F8" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="F8" s="35" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:6" ht="17">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -1852,19 +1857,19 @@
         <v>67</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D9" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" s="35" t="s">
         <v>140</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="F9" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="F9" s="35" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:6" ht="17">
       <c r="A10" t="s">
         <v>68</v>
       </c>
@@ -1872,21 +1877,26 @@
         <v>69</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D10" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="E10" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="F10" s="35" t="s">
         <v>144</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1898,14 +1908,14 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="53.1640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="22.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -1916,7 +1926,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -1924,7 +1934,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -1932,7 +1942,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -1940,7 +1950,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -1948,7 +1958,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -1956,7 +1966,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
@@ -1964,7 +1974,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1972,7 +1982,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -1980,7 +1990,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1988,7 +1998,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -1996,7 +2006,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
@@ -2004,7 +2014,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -2015,25 +2025,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2045,14 +2060,14 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="25.83203125" customWidth="1"/>
     <col min="3" max="3" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="25" t="s">
         <v>77</v>
       </c>
@@ -2063,7 +2078,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -2074,7 +2089,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -2085,64 +2100,69 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2154,12 +2174,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="26" t="s">
         <v>81</v>
       </c>
@@ -2176,7 +2196,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="26" t="s">
         <v>84</v>
       </c>
@@ -2193,7 +2213,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -2213,6 +2233,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2220,11 +2245,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" customWidth="1"/>
@@ -2236,7 +2261,7 @@
     <col min="8" max="8" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="29" t="s">
         <v>91</v>
       </c>
@@ -2262,9 +2287,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="30">
       <c r="A2" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>99</v>
@@ -2282,7 +2307,7 @@
         <v>104</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>105</v>
+        <v>157</v>
       </c>
       <c r="H2" s="32" t="s">
         <v>100</v>
@@ -2291,6 +2316,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2302,13 +2332,13 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.83203125" customWidth="1"/>
     <col min="4" max="4" width="49.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -2322,14 +2352,14 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="24" t="s">
         <v>74</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
     </row>
-    <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="30">
       <c r="A3" s="24" t="s">
         <v>75</v>
       </c>
@@ -2341,5 +2371,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change registration and registrationMember to have required fields and default values
</commit_message>
<xml_diff>
--- a/appGreece/config/tables/registration/forms/registration/registration.xlsx
+++ b/appGreece/config/tables/registration/forms/registration/registration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="3240" windowWidth="34900" windowHeight="19500" tabRatio="994" activeTab="6"/>
+    <workbookView xWindow="-3860" yWindow="1220" windowWidth="50660" windowHeight="21200" tabRatio="994"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="properties" sheetId="8" r:id="rId6"/>
     <sheet name="queries" sheetId="9" r:id="rId7"/>
     <sheet name="initial" sheetId="11" r:id="rId8"/>
+    <sheet name="prompt_types" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="169">
   <si>
     <t>clause</t>
   </si>
@@ -149,12 +150,6 @@
   </si>
   <si>
     <t>hh_size</t>
-  </si>
-  <si>
-    <t>How many people are in your household?</t>
-  </si>
-  <si>
-    <t>Including household representative</t>
   </si>
   <si>
     <t>geopoint</t>
@@ -508,7 +503,46 @@
     <t>text.greek</t>
   </si>
   <si>
-    <t>{beneficiary_code: data('beneficiary_code'), _group_modify: 'hardcodedTestGroup'}</t>
+    <t>async_assign_count</t>
+  </si>
+  <si>
+    <t>count_members</t>
+  </si>
+  <si>
+    <t>prompt_type_name</t>
+  </si>
+  <si>
+    <t>async_assign_max</t>
+  </si>
+  <si>
+    <t>async_assign_min</t>
+  </si>
+  <si>
+    <t>async_assign_avg</t>
+  </si>
+  <si>
+    <t>async_assign_sum</t>
+  </si>
+  <si>
+    <t>async_assign_total</t>
+  </si>
+  <si>
+    <t>async_assign_single_string</t>
+  </si>
+  <si>
+    <t>{beneficiary_code: data('beneficiary_code'), _group_modify: metadata('_group_modify')}</t>
+  </si>
+  <si>
+    <t>!data('tent_caravan')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!data('address') </t>
+  </si>
+  <si>
+    <t>display.required_message.text</t>
+  </si>
+  <si>
+    <t>Either tent/caravan or address must be completed.</t>
   </si>
 </sst>
 </file>
@@ -674,7 +708,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -710,8 +744,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -767,8 +809,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -786,6 +829,10 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -803,6 +850,10 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1205,10 +1256,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" x14ac:dyDescent="0"/>
@@ -1224,9 +1275,10 @@
     <col min="9" max="9" width="30.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="29.1640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="21.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="50.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1260,8 +1312,11 @@
       <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="37" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2" s="2" t="s">
@@ -1280,7 +1335,7 @@
       <c r="J2"/>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3" s="2" t="s">
@@ -1300,7 +1355,7 @@
       <c r="J3"/>
       <c r="K3"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4" s="14" t="s">
@@ -1320,7 +1375,7 @@
       <c r="J4"/>
       <c r="K4"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1335,26 +1390,28 @@
       <c r="J5"/>
       <c r="K5"/>
     </row>
-    <row r="6" spans="1:11" ht="409">
+    <row r="6" spans="1:12" ht="409">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
       <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
-      <c r="K6"/>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -1369,7 +1426,7 @@
       <c r="J7"/>
       <c r="K7"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -1379,7 +1436,7 @@
       <c r="I8"/>
       <c r="J8"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9" s="2" t="s">
@@ -1397,7 +1454,7 @@
       <c r="J9"/>
       <c r="K9"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10" s="2" t="s">
@@ -1419,7 +1476,7 @@
       </c>
       <c r="K10"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1430,13 +1487,13 @@
       <c r="J11"/>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:12">
       <c r="A13"/>
       <c r="C13" s="2" t="s">
         <v>29</v>
@@ -1455,7 +1512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12">
       <c r="A14"/>
       <c r="C14" s="2" t="s">
         <v>18</v>
@@ -1469,28 +1526,33 @@
       <c r="F14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="K14"/>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="K14" t="s">
+        <v>165</v>
+      </c>
+      <c r="L14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15"/>
       <c r="C15" s="2" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K15" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>108</v>
+      </c>
+      <c r="F15" s="12"/>
+      <c r="K15" t="s">
+        <v>166</v>
+      </c>
+      <c r="L15" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -1518,7 +1580,7 @@
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
@@ -1531,16 +1593,16 @@
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I19"/>
       <c r="J19"/>
@@ -1558,31 +1620,52 @@
       <c r="K20"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="C21" s="2" t="s">
+      <c r="A21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="12"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="C22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22"/>
-      <c r="C22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F22" s="12"/>
-      <c r="K22" s="1" t="b">
-        <v>1</v>
-      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="C23" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="H23" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25"/>
+      <c r="F25" s="12"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1612,27 +1695,27 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>44</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="20">
         <v>20170530</v>
@@ -1641,24 +1724,24 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>19</v>
@@ -1691,22 +1774,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" t="s">
         <v>54</v>
-      </c>
-      <c r="B1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17">
@@ -1717,16 +1800,16 @@
         <v>36</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D2" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="35" t="s">
         <v>118</v>
-      </c>
-      <c r="E2" s="35" t="s">
-        <v>119</v>
-      </c>
-      <c r="F2" s="35" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17">
@@ -1734,39 +1817,39 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D3" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="35" t="s">
         <v>121</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="F3" s="35" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D4" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" s="35" t="s">
         <v>124</v>
-      </c>
-      <c r="E4" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="F4" s="35" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17">
@@ -1774,19 +1857,19 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D5" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" s="35" t="s">
         <v>127</v>
-      </c>
-      <c r="E5" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="F5" s="35" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17">
@@ -1794,99 +1877,99 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D6" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" s="35" t="s">
         <v>130</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>131</v>
-      </c>
-      <c r="F6" s="35" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D7" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="35" t="s">
         <v>133</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="F7" s="35" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D8" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="35" t="s">
         <v>136</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="F8" s="35" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D9" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="F9" s="35" t="s">
         <v>139</v>
-      </c>
-      <c r="E9" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="F9" s="35" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D10" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="F10" s="35" t="s">
         <v>142</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1923,7 +2006,7 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1979,7 +2062,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1995,7 +2078,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2008,10 +2091,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2027,10 +2110,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2038,7 +2121,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2069,13 +2152,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2083,10 +2166,10 @@
         <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2094,10 +2177,10 @@
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2105,10 +2188,10 @@
         <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2116,10 +2199,10 @@
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2127,10 +2210,10 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2138,10 +2221,10 @@
         <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2149,10 +2232,10 @@
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2181,53 +2264,53 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>81</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>83</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>84</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>86</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C3" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="26" t="s">
         <v>88</v>
-      </c>
-      <c r="D3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2243,9 +2326,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -2263,54 +2346,80 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="D1" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="E1" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="F1" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="G1" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="H1" s="31" t="s">
         <v>96</v>
-      </c>
-      <c r="G1" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1" s="31" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30">
       <c r="A2" s="24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C2" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="G2" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="F2" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>157</v>
-      </c>
-      <c r="H2" s="32" t="s">
-        <v>100</v>
+      <c r="G3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2346,27 +2455,115 @@
         <v>2</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
     </row>
     <row r="3" spans="1:4" ht="30">
       <c r="A3" s="24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
       <c r="D3" s="24" t="s">
-        <v>76</v>
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="32.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>